<commit_message>
Instruções: Tirar os números dos nomes das ações em programação.xlsx e salvar em texto.txt as infos de interesse como mostrado no script app.py
</commit_message>
<xml_diff>
--- a/programação.xlsx
+++ b/programação.xlsx
@@ -34,7 +34,7 @@
     <t xml:space="preserve">Alváro </t>
   </si>
   <si>
-    <t xml:space="preserve">['AZUL4','GOLL4','CVCB3']</t>
+    <t xml:space="preserve">['AZUL','GOLL','CVCB']</t>
   </si>
   <si>
     <t xml:space="preserve">Gustavo</t>
@@ -218,10 +218,10 @@
   <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.70703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.72265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="11.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="10.12"/>

</xml_diff>